<commit_message>
modified:   data/2024Q4_20250203.xlsx modified:   pages/Q2_2024_Report.py modified:   pages/Q3_2024_Report.py new file:   utils/template.py
</commit_message>
<xml_diff>
--- a/data/2024Q4_20250203.xlsx
+++ b/data/2024Q4_20250203.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nina/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0F98EFC-4C52-424A-99FC-5E57EE21F3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{08B45A3B-71C2-B047-BD07-3C232CF5F13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="500" windowWidth="34000" windowHeight="19360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="criteria for qualitative assess" sheetId="1" r:id="rId1"/>
@@ -323,7 +323,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="185">
   <si>
     <t>date of publication</t>
   </si>
@@ -890,12 +890,6 @@
     <t>Women and men in ICT: a chance for better work-life balance</t>
   </si>
   <si>
-    <t>Document not publicly available</t>
-  </si>
-  <si>
-    <t>Not found</t>
-  </si>
-  <si>
     <t>University of Antwerpen</t>
   </si>
   <si>
@@ -1143,7 +1137,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1188,9 +1182,6 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1427,7 +1418,7 @@
   <dimension ref="A1:AA960"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32"/>
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1525,7 +1516,7 @@
         <v>104</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I2" s="4">
         <v>2023</v>
@@ -1533,7 +1524,7 @@
       <c r="J2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="31" t="s">
         <v>45</v>
       </c>
       <c r="L2" s="4">
@@ -1548,7 +1539,10 @@
       <c r="O2" s="4">
         <v>0</v>
       </c>
-      <c r="P2" s="9"/>
+      <c r="P2" s="9">
+        <f>K4*0.2 + L4*0.4 + M4*0.1 + N4*0.1</f>
+        <v>3.1000000000000005</v>
+      </c>
       <c r="Q2" s="4" t="s">
         <v>25</v>
       </c>
@@ -1583,16 +1577,16 @@
         <v>139</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I3" s="4">
         <v>2017</v>
       </c>
       <c r="J3" s="8"/>
-      <c r="K3" s="32" t="s">
+      <c r="K3" s="31" t="s">
         <v>45</v>
       </c>
       <c r="L3" s="4">
@@ -1607,7 +1601,10 @@
       <c r="O3" s="4">
         <v>0</v>
       </c>
-      <c r="P3" s="9"/>
+      <c r="P3" s="9">
+        <f t="shared" ref="P3:P4" si="0">K5*0.2 + L5*0.4 + M5*0.1 + N5*0.1</f>
+        <v>1.2000000000000002</v>
+      </c>
       <c r="Q3" s="4" t="s">
         <v>25</v>
       </c>
@@ -1636,7 +1633,7 @@
         <v>19</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>20</v>
@@ -1645,15 +1642,15 @@
         <v>21</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="I4" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="I4" s="31" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="32">
+      <c r="K4" s="31">
         <v>2</v>
       </c>
       <c r="L4" s="4">
@@ -1669,8 +1666,8 @@
         <v>24</v>
       </c>
       <c r="P4" s="9">
-        <f t="shared" ref="P4:P11" si="0">K4*0.2 + L4*0.4 + M4*0.1 + N4*0.1</f>
-        <v>3.1000000000000005</v>
+        <f>K6*0.2 + L6*0.4 + M6*0.1 + N6*0.1 + 3*0.2</f>
+        <v>1.8000000000000003</v>
       </c>
       <c r="Q4" s="4" t="s">
         <v>25</v>
@@ -1700,7 +1697,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>20</v>
@@ -1711,13 +1708,13 @@
       <c r="H5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="32" t="s">
         <v>22</v>
       </c>
       <c r="J5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="33">
+      <c r="K5" s="32">
         <v>2</v>
       </c>
       <c r="L5" s="10">
@@ -1733,8 +1730,8 @@
         <v>24</v>
       </c>
       <c r="P5" s="9">
-        <f t="shared" si="0"/>
-        <v>1.2000000000000002</v>
+        <f t="shared" ref="P5:P11" si="1">K7*0.2 + L7*0.4 + M7*0.1 + N7*0.1 + 3*0.2</f>
+        <v>1.8000000000000003</v>
       </c>
       <c r="Q5" s="4" t="s">
         <v>25</v>
@@ -1764,7 +1761,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>20</v>
@@ -1773,15 +1770,15 @@
         <v>28</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="I6" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="I6" s="32" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="33">
+      <c r="K6" s="32">
         <v>2</v>
       </c>
       <c r="L6" s="10">
@@ -1797,8 +1794,8 @@
         <v>24</v>
       </c>
       <c r="P6" s="9">
-        <f t="shared" si="0"/>
-        <v>1.2000000000000002</v>
+        <f t="shared" si="1"/>
+        <v>3.8000000000000007</v>
       </c>
       <c r="Q6" s="4" t="s">
         <v>25</v>
@@ -1828,7 +1825,7 @@
         <v>19</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>20</v>
@@ -1837,15 +1834,15 @@
         <v>29</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="I7" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="I7" s="32" t="s">
         <v>22</v>
       </c>
       <c r="J7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="33">
+      <c r="K7" s="32">
         <v>2</v>
       </c>
       <c r="L7" s="10">
@@ -1861,8 +1858,8 @@
         <v>24</v>
       </c>
       <c r="P7" s="9">
-        <f t="shared" si="0"/>
-        <v>1.2000000000000002</v>
+        <f t="shared" si="1"/>
+        <v>1.8000000000000003</v>
       </c>
       <c r="Q7" s="4" t="s">
         <v>25</v>
@@ -1892,7 +1889,7 @@
         <v>19</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>20</v>
@@ -1901,15 +1898,15 @@
         <v>30</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="I8" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="I8" s="32" t="s">
         <v>22</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="33">
+      <c r="K8" s="32">
         <v>2</v>
       </c>
       <c r="L8" s="10">
@@ -1925,8 +1922,8 @@
         <v>24</v>
       </c>
       <c r="P8" s="9">
-        <f t="shared" si="0"/>
-        <v>3.2000000000000006</v>
+        <f t="shared" si="1"/>
+        <v>1.8000000000000003</v>
       </c>
       <c r="Q8" s="4" t="s">
         <v>25</v>
@@ -1956,7 +1953,7 @@
         <v>19</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>20</v>
@@ -1967,13 +1964,13 @@
       <c r="H9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="33" t="s">
+      <c r="I9" s="32" t="s">
         <v>22</v>
       </c>
       <c r="J9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="33">
+      <c r="K9" s="32">
         <v>2</v>
       </c>
       <c r="L9" s="10">
@@ -1989,8 +1986,8 @@
         <v>24</v>
       </c>
       <c r="P9" s="9">
-        <f t="shared" si="0"/>
-        <v>1.2000000000000002</v>
+        <f t="shared" si="1"/>
+        <v>1.8000000000000003</v>
       </c>
       <c r="Q9" s="4" t="s">
         <v>25</v>
@@ -2020,7 +2017,7 @@
         <v>19</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>20</v>
@@ -2031,13 +2028,13 @@
       <c r="H10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="33" t="s">
+      <c r="I10" s="32" t="s">
         <v>22</v>
       </c>
       <c r="J10" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="33">
+      <c r="K10" s="32">
         <v>2</v>
       </c>
       <c r="L10" s="10">
@@ -2053,8 +2050,8 @@
         <v>24</v>
       </c>
       <c r="P10" s="9">
-        <f t="shared" si="0"/>
-        <v>1.2000000000000002</v>
+        <f t="shared" si="1"/>
+        <v>1.3000000000000003</v>
       </c>
       <c r="Q10" s="4" t="s">
         <v>25</v>
@@ -2084,7 +2081,7 @@
         <v>19</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>20</v>
@@ -2095,13 +2092,13 @@
       <c r="H11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="33" t="s">
+      <c r="I11" s="32" t="s">
         <v>22</v>
       </c>
       <c r="J11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="33">
+      <c r="K11" s="32">
         <v>2</v>
       </c>
       <c r="L11" s="10">
@@ -2117,8 +2114,8 @@
         <v>24</v>
       </c>
       <c r="P11" s="9">
-        <f t="shared" si="0"/>
-        <v>1.2000000000000002</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="Q11" s="4" t="s">
         <v>25</v>
@@ -2159,13 +2156,13 @@
       <c r="H12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="32">
+      <c r="I12" s="31">
         <v>2020</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="35"/>
+      <c r="K12" s="34"/>
       <c r="L12" s="4">
         <v>1</v>
       </c>
@@ -2178,7 +2175,10 @@
       <c r="O12" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="P12" s="9"/>
+      <c r="P12" s="9">
+        <f>K12*0.2 + L12*0.4 + M12*0.1 + N12*0.1 + 1* 0.2</f>
+        <v>0.90000000000000013</v>
+      </c>
       <c r="Q12" s="4" t="s">
         <v>25</v>
       </c>
@@ -2218,11 +2218,11 @@
       <c r="H13" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="I13" s="32"/>
+      <c r="I13" s="31"/>
       <c r="J13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="K13" s="32" t="s">
+      <c r="K13" s="31" t="s">
         <v>38</v>
       </c>
       <c r="L13" s="4"/>
@@ -2231,7 +2231,10 @@
       <c r="O13" s="4">
         <v>0</v>
       </c>
-      <c r="P13" s="9"/>
+      <c r="P13" s="9">
+        <f t="shared" ref="P4:P22" si="2">K13*0.2 + L13*0.4 + M13*0.1 + N13*0.1</f>
+        <v>0.4</v>
+      </c>
       <c r="Q13" s="4" t="s">
         <v>25</v>
       </c>
@@ -2269,20 +2272,23 @@
       <c r="H14" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="I14" s="32">
+      <c r="I14" s="31">
         <v>2018</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K14" s="35"/>
+      <c r="K14" s="34"/>
       <c r="L14" s="4">
         <v>1</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="9"/>
+      <c r="P14" s="9">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
       <c r="Q14" s="4" t="s">
         <v>25</v>
       </c>
@@ -2322,13 +2328,13 @@
       <c r="H15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I15" s="32">
+      <c r="I15" s="31">
         <v>2023</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="32" t="s">
+      <c r="K15" s="31" t="s">
         <v>45</v>
       </c>
       <c r="L15" s="4">
@@ -2341,7 +2347,10 @@
       <c r="O15" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="P15" s="9"/>
+      <c r="P15" s="9">
+        <f>K15*0.2 + L15*0.4 + M15*0.1 + N15*0.1 + 5*0.2</f>
+        <v>2.2999999999999998</v>
+      </c>
       <c r="Q15" s="4" t="s">
         <v>25</v>
       </c>
@@ -2379,15 +2388,15 @@
         <v>111</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="I16" s="32">
+        <v>175</v>
+      </c>
+      <c r="I16" s="31">
         <v>2017</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="35"/>
+      <c r="K16" s="34"/>
       <c r="L16" s="4">
         <v>1</v>
       </c>
@@ -2400,7 +2409,10 @@
       <c r="O16" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="P16" s="9"/>
+      <c r="P16" s="9">
+        <f>K16*0.2 + L16*0.4 + M16*0.1 + N16*0.1 + 11 * 0.2</f>
+        <v>2.9000000000000004</v>
+      </c>
       <c r="Q16" s="4" t="s">
         <v>25</v>
       </c>
@@ -2415,7 +2427,7 @@
       <c r="Z16" s="4"/>
       <c r="AA16" s="4"/>
     </row>
-    <row r="17" spans="1:27" s="28" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" s="27" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="24" t="s">
         <v>110</v>
       </c>
@@ -2428,7 +2440,7 @@
       <c r="D17" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="28" t="s">
         <v>109</v>
       </c>
       <c r="F17" s="24" t="s">
@@ -2438,15 +2450,15 @@
         <v>112</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="I17" s="34">
+        <v>176</v>
+      </c>
+      <c r="I17" s="33">
         <v>2023</v>
       </c>
       <c r="J17" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="35"/>
+      <c r="K17" s="34"/>
       <c r="L17" s="24">
         <v>1</v>
       </c>
@@ -2459,7 +2471,10 @@
       <c r="O17" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="P17" s="27"/>
+      <c r="P17" s="9">
+        <f>K17*0.2 + L17*0.4 + M17*0.1 + N17*0.1 + 11*0.2</f>
+        <v>3</v>
+      </c>
       <c r="Q17" s="4" t="s">
         <v>25</v>
       </c>
@@ -2499,18 +2514,21 @@
       <c r="H18" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="I18" s="32"/>
+      <c r="I18" s="31"/>
       <c r="J18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="32" t="s">
+      <c r="K18" s="31" t="s">
         <v>40</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-      <c r="P18" s="9"/>
+      <c r="P18" s="9">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
       <c r="Q18" s="4" t="s">
         <v>25</v>
       </c>
@@ -2536,13 +2554,13 @@
         <v>94</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>181</v>
       </c>
       <c r="G19" s="21" t="s">
         <v>98</v>
@@ -2550,18 +2568,21 @@
       <c r="H19" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="I19" s="32"/>
+      <c r="I19" s="31"/>
       <c r="J19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="32"/>
+      <c r="K19" s="31"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4">
         <v>0</v>
       </c>
-      <c r="P19" s="9"/>
+      <c r="P19" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="Q19" s="4" t="s">
         <v>95</v>
       </c>
@@ -2601,13 +2622,13 @@
       <c r="H20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I20" s="32" t="s">
+      <c r="I20" s="31" t="s">
         <v>22</v>
       </c>
       <c r="J20" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="K20" s="32" t="s">
+      <c r="K20" s="31" t="s">
         <v>45</v>
       </c>
       <c r="L20" s="4">
@@ -2622,7 +2643,10 @@
       <c r="O20" s="4">
         <v>0</v>
       </c>
-      <c r="P20" s="9"/>
+      <c r="P20" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4000000000000001</v>
+      </c>
       <c r="Q20" s="4" t="s">
         <v>25</v>
       </c>
@@ -2645,30 +2669,30 @@
         <v>44</v>
       </c>
       <c r="C21" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="G21" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>186</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I21" s="32">
+      <c r="I21" s="31">
         <v>2020</v>
       </c>
       <c r="J21" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K21" s="35"/>
+      <c r="K21" s="34"/>
       <c r="L21" s="4">
         <v>1</v>
       </c>
@@ -2681,7 +2705,10 @@
       <c r="O21" s="4">
         <v>0</v>
       </c>
-      <c r="P21" s="9"/>
+      <c r="P21" s="9">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
       <c r="Q21" s="4" t="s">
         <v>25</v>
       </c>
@@ -2721,18 +2748,21 @@
       <c r="H22" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="I22" s="32"/>
+      <c r="I22" s="31"/>
       <c r="J22" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="K22" s="35"/>
+      <c r="K22" s="34"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="P22" s="9"/>
+      <c r="P22" s="9">
+        <f>K22*0.2 + L22*0.4 + M22*0.1 + N22*0.1 + 22*0.2</f>
+        <v>4.4000000000000004</v>
+      </c>
       <c r="Q22" s="4" t="s">
         <v>25</v>
       </c>
@@ -2760,7 +2790,7 @@
       <c r="D23" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E23" s="31"/>
+      <c r="E23" s="30"/>
       <c r="F23" s="4" t="s">
         <v>150</v>
       </c>
@@ -2774,7 +2804,7 @@
       <c r="J23" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="K23" s="35"/>
+      <c r="K23" s="34"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
@@ -2880,10 +2910,8 @@
       <c r="AA26" s="4"/>
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="30"/>
-      <c r="B27" s="4" t="s">
-        <v>170</v>
-      </c>
+      <c r="A27" s="29"/>
+      <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -2912,9 +2940,7 @@
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="21"/>
-      <c r="B28" s="4" t="s">
-        <v>169</v>
-      </c>
+      <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>

</xml_diff>